<commit_message>
create new BERT model building
</commit_message>
<xml_diff>
--- a/output_training_model_manually.xlsx
+++ b/output_training_model_manually.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,10 +554,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>132</v>
+        <v>321</v>
       </c>
       <c r="B6" t="n">
-        <v>135</v>
+        <v>330</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -566,7 +566,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>informant</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -577,10 +577,10 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>321</v>
+        <v>74</v>
       </c>
       <c r="B7" t="n">
-        <v>330</v>
+        <v>78</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -589,21 +589,21 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>informant</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>NCT00236431.json</t>
+          <t>NCT00236574.json</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="B8" t="n">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -612,7 +612,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>mild</t>
+          <t>delayed</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -623,10 +623,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>100</v>
+        <v>339</v>
       </c>
       <c r="B9" t="n">
-        <v>107</v>
+        <v>348</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -635,7 +635,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>delayed</t>
+          <t>informant</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -646,10 +646,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>149</v>
+        <v>1066</v>
       </c>
       <c r="B10" t="n">
-        <v>152</v>
+        <v>1070</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -658,21 +658,21 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>NCT00236574.json</t>
+          <t>NCT00265148.json</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>339</v>
+        <v>1764</v>
       </c>
       <c r="B11" t="n">
-        <v>348</v>
+        <v>1767</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -681,21 +681,21 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>informant</t>
+          <t>due</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>NCT00236574.json</t>
+          <t>NCT00265148.json</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1066</v>
+        <v>426</v>
       </c>
       <c r="B12" t="n">
-        <v>1070</v>
+        <v>430</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -709,16 +709,16 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>NCT00265148.json</t>
+          <t>NCT00348140.json</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1764</v>
+        <v>2927</v>
       </c>
       <c r="B13" t="n">
-        <v>1767</v>
+        <v>2930</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -732,16 +732,16 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>NCT00265148.json</t>
+          <t>NCT00348140.json</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>86</v>
+        <v>625</v>
       </c>
       <c r="B14" t="n">
-        <v>92</v>
+        <v>629</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -750,21 +750,21 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>nincds</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>NCT00309725.json</t>
+          <t>NCT00357357.json</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>426</v>
+        <v>159</v>
       </c>
       <c r="B15" t="n">
-        <v>430</v>
+        <v>163</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -778,16 +778,16 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NCT00348140.json</t>
+          <t>NCT00380302.json</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2927</v>
+        <v>1088</v>
       </c>
       <c r="B16" t="n">
-        <v>2930</v>
+        <v>1091</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -801,16 +801,16 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>NCT00348140.json</t>
+          <t>NCT00381238.json</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>625</v>
+        <v>177</v>
       </c>
       <c r="B17" t="n">
-        <v>629</v>
+        <v>181</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -824,16 +824,16 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>NCT00357357.json</t>
+          <t>NCT00384423.json</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>159</v>
+        <v>97</v>
       </c>
       <c r="B18" t="n">
-        <v>163</v>
+        <v>101</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -847,16 +847,16 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>NCT00380302.json</t>
+          <t>NCT00438568.json</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>194</v>
+        <v>89</v>
       </c>
       <c r="B19" t="n">
-        <v>197</v>
+        <v>93</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -865,21 +865,21 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>NCT00380302.json</t>
+          <t>NCT00663936.json</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1088</v>
+        <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>1091</v>
+        <v>24</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -888,21 +888,21 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>due</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>NCT00381238.json</t>
+          <t>NCT00930059.json</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="B21" t="n">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -911,21 +911,21 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>NCT00428090.json</t>
+          <t>NCT01303744.json</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>89</v>
+        <v>904</v>
       </c>
       <c r="B22" t="n">
-        <v>93</v>
+        <v>907</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -934,21 +934,21 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>mild</t>
+          <t>due</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>NCT00663936.json</t>
+          <t>NCT01436045.json</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1262</v>
+        <v>74</v>
       </c>
       <c r="B23" t="n">
-        <v>1265</v>
+        <v>78</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -957,21 +957,21 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>NCT00672945.json</t>
+          <t>NCT01466088.json</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="B24" t="n">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>NCT00930059.json</t>
+          <t>NCT01569516.json</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>760</v>
+        <v>429</v>
       </c>
       <c r="B25" t="n">
-        <v>763</v>
+        <v>433</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1003,21 +1003,21 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>NCT01058941.json</t>
+          <t>NCT01676935.json</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>543</v>
+        <v>347</v>
       </c>
       <c r="B26" t="n">
-        <v>546</v>
+        <v>351</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1026,21 +1026,21 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>did</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>NCT01245530.json</t>
+          <t>NCT01852110.json</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>546</v>
+        <v>530</v>
       </c>
       <c r="B27" t="n">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1049,21 +1049,21 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>n't</t>
+          <t>informant</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>NCT01245530.json</t>
+          <t>NCT01852110.json</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>233</v>
+        <v>398</v>
       </c>
       <c r="B28" t="n">
-        <v>236</v>
+        <v>402</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1072,21 +1072,21 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>NCT01249196.json</t>
+          <t>NCT01940952.json</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>58</v>
+        <v>708</v>
       </c>
       <c r="B29" t="n">
-        <v>62</v>
+        <v>712</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1100,16 +1100,16 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>NCT01303744.json</t>
+          <t>NCT01998841.json</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>904</v>
+        <v>103</v>
       </c>
       <c r="B30" t="n">
-        <v>907</v>
+        <v>107</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1118,21 +1118,21 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>due</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>NCT01436045.json</t>
+          <t>NCT02017340.json</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="B31" t="n">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1146,16 +1146,16 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>NCT01466088.json</t>
+          <t>NCT02284906.json</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>145</v>
+        <v>333</v>
       </c>
       <c r="B32" t="n">
-        <v>149</v>
+        <v>337</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1169,16 +1169,16 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>NCT01569516.json</t>
+          <t>NCT02322021.json</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1079</v>
+        <v>560</v>
       </c>
       <c r="B33" t="n">
-        <v>1082</v>
+        <v>569</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1187,21 +1187,21 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>informant</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>NCT01676935.json</t>
+          <t>NCT02322021.json</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>347</v>
+        <v>78</v>
       </c>
       <c r="B34" t="n">
-        <v>351</v>
+        <v>82</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1215,16 +1215,16 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>NCT01852110.json</t>
+          <t>NCT02423122.json</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B35" t="n">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1238,16 +1238,16 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>NCT01852110.json</t>
+          <t>NCT02484547.json</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>398</v>
+        <v>20</v>
       </c>
       <c r="B36" t="n">
-        <v>402</v>
+        <v>24</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1261,16 +1261,16 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>NCT01940952.json</t>
+          <t>NCT02646982.json</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>708</v>
+        <v>314</v>
       </c>
       <c r="B37" t="n">
-        <v>712</v>
+        <v>318</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1284,16 +1284,16 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>NCT01998841.json</t>
+          <t>NCT02907567.json</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>3110</v>
+        <v>289</v>
       </c>
       <c r="B38" t="n">
-        <v>3113</v>
+        <v>293</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1302,21 +1302,21 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>NCT01998841.json</t>
+          <t>NCT02997982.json</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3325</v>
+        <v>315</v>
       </c>
       <c r="B39" t="n">
-        <v>3328</v>
+        <v>318</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1325,21 +1325,21 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>due</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>NCT01998841.json</t>
+          <t>NCT02997982.json</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>3598</v>
+        <v>154</v>
       </c>
       <c r="B40" t="n">
-        <v>3601</v>
+        <v>158</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1348,12 +1348,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>NCT01998841.json</t>
+          <t>NCT03352557.json</t>
         </is>
       </c>
     </row>
@@ -1376,16 +1376,16 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>NCT02017340.json</t>
+          <t>NCT03533257.json</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>423</v>
+        <v>304</v>
       </c>
       <c r="B42" t="n">
-        <v>426</v>
+        <v>308</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1394,21 +1394,21 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>NCT02017340.json</t>
+          <t>NCT04187547.json</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>353</v>
+        <v>3198</v>
       </c>
       <c r="B43" t="n">
-        <v>362</v>
+        <v>3201</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1417,21 +1417,21 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>informant</t>
+          <t>due</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>NCT02033941.json</t>
+          <t>NCT04187547.json</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>390</v>
+        <v>316</v>
       </c>
       <c r="B44" t="n">
-        <v>393</v>
+        <v>320</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1440,21 +1440,21 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>NCT02167256.json</t>
+          <t>NCT04249869.json</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>736</v>
+        <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>739</v>
+        <v>47</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1463,21 +1463,21 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>NCT02167256.json</t>
+          <t>NCT04491006.json</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1107</v>
+        <v>20</v>
       </c>
       <c r="B46" t="n">
-        <v>1110</v>
+        <v>24</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1486,21 +1486,21 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>NCT02167256.json</t>
+          <t>NCT04520412.json</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1684</v>
+        <v>240</v>
       </c>
       <c r="B47" t="n">
-        <v>1687</v>
+        <v>247</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1509,21 +1509,21 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>delayed</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>NCT02246075.json</t>
+          <t>NCT04629495.json</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>333</v>
+        <v>833</v>
       </c>
       <c r="B48" t="n">
-        <v>337</v>
+        <v>837</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1537,16 +1537,16 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>NCT02322021.json</t>
+          <t>NCT04639050.json</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>560</v>
+        <v>1072</v>
       </c>
       <c r="B49" t="n">
-        <v>569</v>
+        <v>1076</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1555,21 +1555,21 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>informant</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>NCT02322021.json</t>
+          <t>NCT04639050.json</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>853</v>
+        <v>1098</v>
       </c>
       <c r="B50" t="n">
-        <v>855</v>
+        <v>1101</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1578,21 +1578,21 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>due</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>NCT02322021.json</t>
+          <t>NCT04639050.json</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>20</v>
+        <v>272</v>
       </c>
       <c r="B51" t="n">
-        <v>24</v>
+        <v>276</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1606,16 +1606,16 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>NCT02646982.json</t>
+          <t>NCT04780399.json</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>209</v>
+        <v>132</v>
       </c>
       <c r="B52" t="n">
-        <v>212</v>
+        <v>141</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1624,21 +1624,21 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>informant</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>NCT02788513.json</t>
+          <t>NCT04902703.json</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>315</v>
+        <v>65</v>
       </c>
       <c r="B53" t="n">
-        <v>318</v>
+        <v>69</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1647,21 +1647,21 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>due</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>NCT02997982.json</t>
+          <t>NCT05006781.json</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="B54" t="n">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1675,16 +1675,16 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>NCT03352557.json</t>
+          <t>NCT05104463.json</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>557</v>
+        <v>20</v>
       </c>
       <c r="B55" t="n">
-        <v>566</v>
+        <v>24</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1693,21 +1693,21 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>informant</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>NCT03352557.json</t>
+          <t>NCT05282550.json</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>398</v>
+        <v>792</v>
       </c>
       <c r="B56" t="n">
-        <v>401</v>
+        <v>801</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1716,21 +1716,21 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>informant</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>NCT03363269.json</t>
+          <t>NCT05282550.json</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>884</v>
+        <v>668</v>
       </c>
       <c r="B57" t="n">
-        <v>886</v>
+        <v>677</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1739,21 +1739,21 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>informant</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>NCT03656042.json</t>
+          <t>NCT05468073.json</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>246</v>
+        <v>124</v>
       </c>
       <c r="B58" t="n">
-        <v>248</v>
+        <v>128</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>m2</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>NCT04063124.json</t>
+          <t>NCT05531526.json</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>629</v>
+        <v>153</v>
       </c>
       <c r="B59" t="n">
-        <v>632</v>
+        <v>157</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1785,21 +1785,21 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>inr</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>NCT04063124.json</t>
+          <t>NCT05531526.json</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1687</v>
+        <v>101</v>
       </c>
       <c r="B60" t="n">
-        <v>1690</v>
+        <v>110</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1808,21 +1808,21 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>not</t>
+          <t>informant</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>NCT04187547.json</t>
+          <t>NCT05738486.json</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>3198</v>
+        <v>1166</v>
       </c>
       <c r="B61" t="n">
-        <v>3201</v>
+        <v>1173</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1831,654 +1831,10 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>due</t>
+          <t>delayed</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
-        <is>
-          <t>NCT04187547.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>848</v>
-      </c>
-      <c r="B62" t="n">
-        <v>851</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>NCT04314934.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>20</v>
-      </c>
-      <c r="B63" t="n">
-        <v>24</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>mild</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>NCT04520412.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>1119</v>
-      </c>
-      <c r="B64" t="n">
-        <v>1122</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>NCT04592341.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>1260</v>
-      </c>
-      <c r="B65" t="n">
-        <v>1263</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>NCT04592341.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>240</v>
-      </c>
-      <c r="B66" t="n">
-        <v>247</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>delayed</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>NCT04629495.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>833</v>
-      </c>
-      <c r="B67" t="n">
-        <v>837</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>mild</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>NCT04639050.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>879</v>
-      </c>
-      <c r="B68" t="n">
-        <v>887</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>national</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>NCT04639050.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>1098</v>
-      </c>
-      <c r="B69" t="n">
-        <v>1101</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>due</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>NCT04639050.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>1565</v>
-      </c>
-      <c r="B70" t="n">
-        <v>1568</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>NCT04639050.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>1705</v>
-      </c>
-      <c r="B71" t="n">
-        <v>1708</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>NCT04639050.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>272</v>
-      </c>
-      <c r="B72" t="n">
-        <v>276</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>mild</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>NCT04780399.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>132</v>
-      </c>
-      <c r="B73" t="n">
-        <v>141</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>informant</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>NCT04902703.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>590</v>
-      </c>
-      <c r="B74" t="n">
-        <v>593</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>NCT04902703.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>1835</v>
-      </c>
-      <c r="B75" t="n">
-        <v>1838</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>NCT05104463.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>20</v>
-      </c>
-      <c r="B76" t="n">
-        <v>24</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>mild</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>NCT05282550.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>235</v>
-      </c>
-      <c r="B77" t="n">
-        <v>236</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>;</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>NCT05282550.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>792</v>
-      </c>
-      <c r="B78" t="n">
-        <v>801</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>informant</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>NCT05282550.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>164</v>
-      </c>
-      <c r="B79" t="n">
-        <v>167</v>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>NCT05468073.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>668</v>
-      </c>
-      <c r="B80" t="n">
-        <v>677</v>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>informant</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>NCT05468073.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>681</v>
-      </c>
-      <c r="B81" t="n">
-        <v>684</v>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>NCT05468073.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>271</v>
-      </c>
-      <c r="B82" t="n">
-        <v>274</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>NCT05476783.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>124</v>
-      </c>
-      <c r="B83" t="n">
-        <v>128</v>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>mild</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>NCT05531526.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>574</v>
-      </c>
-      <c r="B84" t="n">
-        <v>581</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>delayed</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>NCT05531526.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>1757</v>
-      </c>
-      <c r="B85" t="n">
-        <v>1760</v>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>NCT05686044.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>1968</v>
-      </c>
-      <c r="B86" t="n">
-        <v>1971</v>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>NCT05686044.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>3484</v>
-      </c>
-      <c r="B87" t="n">
-        <v>3487</v>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>not</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>NCT05686044.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>1166</v>
-      </c>
-      <c r="B88" t="n">
-        <v>1173</v>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>delayed</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>NCT05986721.json</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>2238</v>
-      </c>
-      <c r="B89" t="n">
-        <v>2240</v>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>caregiver</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
         <is>
           <t>NCT05986721.json</t>
         </is>

</xml_diff>